<commit_message>
modified seasonal transition signature (debugged initial values, discard unstable first-year estimate, options to return transition dates in datetime)
</commit_message>
<xml_diff>
--- a/2_data_input/Mahurangi/parameters/ex1_GLUE_config.xlsx
+++ b/2_data_input/Mahurangi/parameters/ex1_GLUE_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\Ryoko and Hilary\SMSigxModel\analysis\2_data_input\Mahurangi\parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C608A8B-5EE7-4475-BE0F-A04F4C3C1469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DAD63D3-8C6D-42B1-BE2C-86C948A53D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,11 +100,11 @@
     <t>lksatfac</t>
   </si>
   <si>
-    <t>trigger_z_m_coeff</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>K_nash</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>trigger_z_fact</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -434,7 +434,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -586,7 +586,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B11">
         <v>0.25</v>
@@ -656,7 +656,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16">
         <v>0</v>

</xml_diff>

<commit_message>
Multiprocessing -> Pool method
</commit_message>
<xml_diff>
--- a/2_data_input/Mahurangi/parameters/ex1_GLUE_config.xlsx
+++ b/2_data_input/Mahurangi/parameters/ex1_GLUE_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\Ryoko and Hilary\SMSigxModel\analysis\2_data_input\Mahurangi\parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DAD63D3-8C6D-42B1-BE2C-86C948A53D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C201D55-4CD6-436C-B898-3C1DC75CD386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -434,7 +434,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -519,7 +519,7 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -536,7 +536,7 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
       <c r="D7">
         <v>1</v>

</xml_diff>

<commit_message>
Changed the window size and parameters for seasonal transition signature
</commit_message>
<xml_diff>
--- a/2_data_input/Mahurangi/parameters/ex1_GLUE_config.xlsx
+++ b/2_data_input/Mahurangi/parameters/ex1_GLUE_config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\Ryoko and Hilary\SMSigxModel\analysis\2_data_input\Mahurangi\parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C201D55-4CD6-436C-B898-3C1DC75CD386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1EBE36-7424-434B-B89B-787D0C7B924A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -434,7 +434,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -631,10 +631,10 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="C14">
-        <v>8</v>
+        <v>0.1</v>
       </c>
       <c r="D14">
         <v>1</v>

</xml_diff>

<commit_message>
Better plot for posters
</commit_message>
<xml_diff>
--- a/2_data_input/Mahurangi/parameters/ex1_GLUE_config.xlsx
+++ b/2_data_input/Mahurangi/parameters/ex1_GLUE_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\Ryoko and Hilary\SMSigxModel\analysis\2_data_input\Mahurangi\parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1EBE36-7424-434B-B89B-787D0C7B924A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E337FA7-8BF1-401F-B4BB-E35287E6D924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1410" yWindow="1350" windowWidth="15375" windowHeight="7950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -433,8 +433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -631,10 +631,10 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="C14">
-        <v>0.1</v>
+        <v>8</v>
       </c>
       <c r="D14">
         <v>1</v>

</xml_diff>